<commit_message>
checkout point to add testing and see if it works on remote (local testing not working)
</commit_message>
<xml_diff>
--- a/exposan/pou_disinfection/data/impact_items.xlsx
+++ b/exposan/pou_disinfection/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\EXPOsan\exposan\pou_disinfection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A599C9-5631-423D-B90A-BCF006CAA4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD889F2-1510-43F6-9197-B42E71EA06BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="19200" windowHeight="11170" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
+    <workbookView xWindow="260" yWindow="2040" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -102,13 +102,31 @@
   </si>
   <si>
     <t>UVlamp</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>ImpactItem</t>
+  </si>
+  <si>
+    <t>StreamImpactItem</t>
+  </si>
+  <si>
+    <t>NaClO</t>
+  </si>
+  <si>
+    <t>kind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +148,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,10 +177,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD9C950-177D-4B3A-BB21-99D6C3BED303}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,92 +508,147 @@
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F9C3F1-FB43-4A86-A175-721791A0658A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,255 +671,303 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
         <v>4.33</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>3.07</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>5.5</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
         <v>2.7932999999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>2.0949749999999998</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>3.491625</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
         <v>2.4203999999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>1.8152999999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>3.0255000000000001</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.98118000000000005</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>0.73588500000000001</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>1.226475</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
         <v>15.106</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>11.329499999999999</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>18.8825</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
         <v>1.0238000000000001E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>7.6785000000000004E-3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>1.27975E-2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
         <v>496.58</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>372.435</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>620.72500000000002</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
         <v>2.2008E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>1.6506E-2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>2.751E-2</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
         <v>3.5012000000000001E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>2.6259000000000001E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>4.3764999999999998E-2</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
         <v>247.43</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>185.57249999999999</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>309.17500000000001</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1135</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.106</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.121</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2.6286999999999998</v>
+      </c>
+      <c r="D13">
+        <f>$C13*0.75</f>
+        <v>1.9715249999999997</v>
+      </c>
+      <c r="E13">
+        <f>$C13*1.25</f>
+        <v>3.2858749999999999</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates in response to issue #39
</commit_message>
<xml_diff>
--- a/exposan/pou_disinfection/data/impact_items.xlsx
+++ b/exposan/pou_disinfection/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\EXPOsan\exposan\pou_disinfection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD889F2-1510-43F6-9197-B42E71EA06BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFB3822-0231-4609-8052-E9518E168EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="2040" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
+    <workbookView xWindow="3797" yWindow="1037" windowWidth="22080" windowHeight="15686" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>kind</t>
+  </si>
+  <si>
+    <t>PE_stream</t>
   </si>
 </sst>
 </file>
@@ -177,11 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -497,29 +498,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD9C950-177D-4B3A-BB21-99D6C3BED303}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -530,7 +531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -541,7 +542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -552,7 +553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -563,7 +564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -574,7 +575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -585,7 +586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -596,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -607,7 +608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -618,7 +619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -629,7 +630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -640,7 +641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -648,6 +649,18 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B3</f>
+        <v>kg</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -658,299 +671,299 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F9C3F1-FB43-4A86-A175-721791A0658A}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.15234375" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>4.33</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>3.07</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>5.5</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>2.7932999999999999</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>2.0949749999999998</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>3.491625</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>2.4203999999999999</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>1.8152999999999999</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>3.0255000000000001</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>0.98118000000000005</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>0.73588500000000001</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>1.226475</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>15.106</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>11.329499999999999</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>18.8825</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>1.0238000000000001E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>7.6785000000000004E-3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>1.27975E-2</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>496.58</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>372.435</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>620.72500000000002</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
         <v>2.2008E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>1.6506E-2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>2.751E-2</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
         <v>3.5012000000000001E-2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>2.6259000000000001E-2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>4.3764999999999998E-2</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
         <v>247.43</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>185.57249999999999</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>309.17500000000001</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
         <v>0.1135</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>0.106</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>0.121</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13">
@@ -964,11 +977,39 @@
         <f>$C13*1.25</f>
         <v>3.2858749999999999</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>9</v>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f>C3</f>
+        <v>2.7932999999999999</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:G14" si="0">D3</f>
+        <v>2.0949749999999998</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3.491625</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>uniform</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>ecoinvent 3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update electricity and stainless steel CF for #39
</commit_message>
<xml_diff>
--- a/exposan/pou_disinfection/data/impact_items.xlsx
+++ b/exposan/pou_disinfection/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\EXPOsan\exposan\pou_disinfection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFB3822-0231-4609-8052-E9518E168EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311BBD37-A200-4770-96DB-8A64FB058CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3797" yWindow="1037" windowWidth="22080" windowHeight="15686" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
+    <workbookView xWindow="7620" yWindow="1209" windowWidth="21746" windowHeight="16208" activeTab="1" xr2:uid="{66280BDC-8972-43BC-9664-C5F2FA84B674}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -500,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD9C950-177D-4B3A-BB21-99D6C3BED303}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F9C3F1-FB43-4A86-A175-721791A0658A}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -714,13 +714,15 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>4.33</v>
+        <v>5.0231000000000003</v>
       </c>
       <c r="D2">
-        <v>3.07</v>
+        <f>$C2*0.75</f>
+        <v>3.7673250000000005</v>
       </c>
       <c r="E2">
-        <v>5.5</v>
+        <f>$C2*1.25</f>
+        <v>6.2788750000000002</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -944,13 +946,15 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>0.1135</v>
+        <v>0.69711999999999996</v>
       </c>
       <c r="D12">
-        <v>0.106</v>
+        <f>$C12*0.75</f>
+        <v>0.52283999999999997</v>
       </c>
       <c r="E12">
-        <v>0.121</v>
+        <f>$C12*1.25</f>
+        <v>0.87139999999999995</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>

</xml_diff>